<commit_message>
All ADC channels have been tested and are functional
</commit_message>
<xml_diff>
--- a/EEPROM_Management.xlsx
+++ b/EEPROM_Management.xlsx
@@ -10,7 +10,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>EEPROM:</t>
   </si>
@@ -86,6 +85,18 @@
   </si>
   <si>
     <t>Air to fuel ratio ADC vector 1024x1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Throttle position sensor Low (engine_config) 8 bits </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Throttle position sensor high (engine_config) 8 bits </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manifold absolute pressure high (engine_config) 8 bits </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manifold absolute pressure Low (engine_config) 8 bits </t>
   </si>
 </sst>
 </file>
@@ -417,7 +428,7 @@
   <dimension ref="A1:D98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,824 +669,848 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
       <c r="B17">
         <f t="shared" si="0"/>
         <v>3936</v>
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
-        <v>3935</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+        <v>3936</v>
+      </c>
+      <c r="D17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3937</v>
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
-        <v>3935</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+        <v>3937</v>
+      </c>
+      <c r="D18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3938</v>
       </c>
       <c r="C19">
         <f t="shared" si="1"/>
-        <v>3935</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+        <v>3938</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2</v>
+      </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3939</v>
       </c>
       <c r="C20">
         <f t="shared" si="1"/>
-        <v>3935</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+        <v>3940</v>
+      </c>
+      <c r="D20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C21">
         <f t="shared" si="1"/>
-        <v>3935</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+        <v>3940</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C22">
         <f t="shared" si="1"/>
-        <v>3935</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+        <v>3940</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C23">
         <f t="shared" si="1"/>
-        <v>3935</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+        <v>3940</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C24">
         <f t="shared" si="1"/>
-        <v>3935</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+        <v>3940</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C25">
         <f t="shared" si="1"/>
-        <v>3935</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+        <v>3940</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C26">
         <f t="shared" si="1"/>
-        <v>3935</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+        <v>3940</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C27">
         <f t="shared" si="1"/>
-        <v>3935</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+        <v>3940</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C28">
         <f t="shared" si="1"/>
-        <v>3935</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+        <v>3940</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C29">
         <f t="shared" si="1"/>
-        <v>3935</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+        <v>3940</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C30">
         <f t="shared" si="1"/>
-        <v>3935</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+        <v>3940</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C31">
         <f t="shared" si="1"/>
-        <v>3935</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+        <v>3940</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C32">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C33">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C34">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C35">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C36">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C37">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C38">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C39">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C40">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C41">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C42">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C43">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C44">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C45">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C46">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C47">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C48">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C49">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C50">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C51">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C52">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C53">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C54">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C55">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C56">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C57">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C58">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C59">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C60">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C61">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C62">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C63">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C64">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C65">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C66">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C67">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C68">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C69">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70">
         <f t="shared" si="0"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C70">
         <f t="shared" si="1"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71">
         <f t="shared" ref="B71:B98" si="2">C70+1</f>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C71">
         <f t="shared" ref="C71:C98" si="3">B71+A71-1</f>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72">
         <f t="shared" si="2"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C72">
         <f t="shared" si="3"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73">
         <f t="shared" si="2"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C73">
         <f t="shared" si="3"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74">
         <f t="shared" si="2"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C74">
         <f t="shared" si="3"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75">
         <f t="shared" si="2"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C75">
         <f t="shared" si="3"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76">
         <f t="shared" si="2"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C76">
         <f t="shared" si="3"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77">
         <f t="shared" si="2"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C77">
         <f t="shared" si="3"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78">
         <f t="shared" si="2"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C78">
         <f t="shared" si="3"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79">
         <f t="shared" si="2"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C79">
         <f t="shared" si="3"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80">
         <f t="shared" si="2"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C80">
         <f t="shared" si="3"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81">
         <f t="shared" si="2"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C81">
         <f t="shared" si="3"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82">
         <f t="shared" si="2"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C82">
         <f t="shared" si="3"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83">
         <f t="shared" si="2"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C83">
         <f t="shared" si="3"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84">
         <f t="shared" si="2"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C84">
         <f t="shared" si="3"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85">
         <f t="shared" si="2"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C85">
         <f t="shared" si="3"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86">
         <f t="shared" si="2"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C86">
         <f t="shared" si="3"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87">
         <f t="shared" si="2"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C87">
         <f t="shared" si="3"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88">
         <f t="shared" si="2"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C88">
         <f t="shared" si="3"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89">
         <f t="shared" si="2"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C89">
         <f t="shared" si="3"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90">
         <f t="shared" si="2"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C90">
         <f t="shared" si="3"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91">
         <f t="shared" si="2"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C91">
         <f t="shared" si="3"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92">
         <f t="shared" si="2"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C92">
         <f t="shared" si="3"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93">
         <f t="shared" si="2"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C93">
         <f t="shared" si="3"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94">
         <f t="shared" si="2"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C94">
         <f t="shared" si="3"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95">
         <f t="shared" si="2"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C95">
         <f t="shared" si="3"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96">
         <f t="shared" si="2"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C96">
         <f t="shared" si="3"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97">
         <f t="shared" si="2"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C97">
         <f t="shared" si="3"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98">
         <f t="shared" si="2"/>
-        <v>3936</v>
+        <v>3941</v>
       </c>
       <c r="C98">
         <f t="shared" si="3"/>
-        <v>3935</v>
+        <v>3940</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished configuring tunerstudio .ini file
It is needed to create structs of config variables which are the same as
in .ini file
</commit_message>
<xml_diff>
--- a/EEPROM_Management.xlsx
+++ b/EEPROM_Management.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17668"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>EEPROM:</t>
   </si>
@@ -93,10 +93,13 @@
     <t xml:space="preserve">Throttle position sensor high (engine_config) 8 bits </t>
   </si>
   <si>
-    <t xml:space="preserve">Manifold absolute pressure high (engine_config) 8 bits </t>
-  </si>
-  <si>
     <t xml:space="preserve">Manifold absolute pressure Low (engine_config) 8 bits </t>
+  </si>
+  <si>
+    <t>Injector opening time (engine_config) 8 bits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manifold absolute pressure high (engine_config) 16 bits </t>
   </si>
 </sst>
 </file>
@@ -428,7 +431,7 @@
   <dimension ref="A1:D98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,7 +717,7 @@
         <v>3938</v>
       </c>
       <c r="D19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -730,787 +733,793 @@
         <v>3940</v>
       </c>
       <c r="D20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
       <c r="B21">
         <f t="shared" si="0"/>
         <v>3941</v>
       </c>
       <c r="C21">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
+      </c>
+      <c r="D21" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C22">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C23">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C24">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C25">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C26">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C27">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C28">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C29">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C30">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C31">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C32">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C33">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C34">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C35">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C36">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C37">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C38">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C39">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C40">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C41">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C42">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C43">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C44">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C45">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C46">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C47">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C48">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C49">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C50">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C51">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C52">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C53">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C54">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C55">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C56">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C57">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C58">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C59">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C60">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C61">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C62">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C63">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C64">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C65">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C66">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C67">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C68">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C69">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70">
         <f t="shared" si="0"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C70">
         <f t="shared" si="1"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71">
         <f t="shared" ref="B71:B98" si="2">C70+1</f>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C71">
         <f t="shared" ref="C71:C98" si="3">B71+A71-1</f>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72">
         <f t="shared" si="2"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C72">
         <f t="shared" si="3"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73">
         <f t="shared" si="2"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C73">
         <f t="shared" si="3"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74">
         <f t="shared" si="2"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C74">
         <f t="shared" si="3"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75">
         <f t="shared" si="2"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C75">
         <f t="shared" si="3"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76">
         <f t="shared" si="2"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C76">
         <f t="shared" si="3"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77">
         <f t="shared" si="2"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C77">
         <f t="shared" si="3"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78">
         <f t="shared" si="2"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C78">
         <f t="shared" si="3"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79">
         <f t="shared" si="2"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C79">
         <f t="shared" si="3"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80">
         <f t="shared" si="2"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C80">
         <f t="shared" si="3"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81">
         <f t="shared" si="2"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C81">
         <f t="shared" si="3"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82">
         <f t="shared" si="2"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C82">
         <f t="shared" si="3"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83">
         <f t="shared" si="2"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C83">
         <f t="shared" si="3"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84">
         <f t="shared" si="2"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C84">
         <f t="shared" si="3"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85">
         <f t="shared" si="2"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C85">
         <f t="shared" si="3"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86">
         <f t="shared" si="2"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C86">
         <f t="shared" si="3"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87">
         <f t="shared" si="2"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C87">
         <f t="shared" si="3"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88">
         <f t="shared" si="2"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C88">
         <f t="shared" si="3"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89">
         <f t="shared" si="2"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C89">
         <f t="shared" si="3"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90">
         <f t="shared" si="2"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C90">
         <f t="shared" si="3"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91">
         <f t="shared" si="2"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C91">
         <f t="shared" si="3"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92">
         <f t="shared" si="2"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C92">
         <f t="shared" si="3"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93">
         <f t="shared" si="2"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C93">
         <f t="shared" si="3"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94">
         <f t="shared" si="2"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C94">
         <f t="shared" si="3"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95">
         <f t="shared" si="2"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C95">
         <f t="shared" si="3"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96">
         <f t="shared" si="2"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C96">
         <f t="shared" si="3"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97">
         <f t="shared" si="2"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C97">
         <f t="shared" si="3"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98">
         <f t="shared" si="2"/>
-        <v>3941</v>
+        <v>3942</v>
       </c>
       <c r="C98">
         <f t="shared" si="3"/>
-        <v>3940</v>
+        <v>3941</v>
       </c>
     </row>
   </sheetData>

</xml_diff>